<commit_message>
feat: adding knowledge database to ai
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauricio.santos\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauricio.santos\Desktop\gruposc.ia\sup sistemas ia\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="103">
   <si>
     <t>processo</t>
   </si>
@@ -312,7 +312,32 @@
     <t>descricao</t>
   </si>
   <si>
-    <t>Emissão de NFI (Nota Fiscal de Incineração)</t>
+    <t>Classificação e determinação de NFOs</t>
+  </si>
+  <si>
+    <t>Monitor de compras, onde é gerado a id agrupamento</t>
+  </si>
+  <si>
+    <t>Monitor fiscal para Ids, onde é gerado o espelho para emissão da NFD</t>
+  </si>
+  <si>
+    <t>101 - avaria interna
+102 - avaria externa
+108 - avaria Cross
+013 - avaria fob
+113 - avaria comercial</t>
+  </si>
+  <si>
+    <t>explicacao</t>
+  </si>
+  <si>
+    <t>depositos</t>
+  </si>
+  <si>
+    <t>Emissão de NF Devolução (NFD)</t>
+  </si>
+  <si>
+    <t>Emissão de NF de Incineração (NFI)</t>
   </si>
 </sst>
 </file>
@@ -348,8 +373,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -641,9 +669,10 @@
     <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -653,8 +682,11 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -665,7 +697,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -675,8 +707,11 @@
       <c r="C3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -687,7 +722,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -698,7 +733,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -709,7 +744,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -720,7 +755,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -731,7 +766,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -742,7 +777,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -753,7 +788,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -764,7 +799,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -775,7 +810,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -786,7 +821,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -797,7 +832,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -808,7 +843,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -819,7 +854,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -830,7 +865,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -841,7 +876,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -852,7 +887,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -863,7 +898,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -873,8 +908,11 @@
       <c r="C21" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -884,8 +922,11 @@
       <c r="C22" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -895,8 +936,11 @@
       <c r="C23" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -907,7 +951,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -918,7 +962,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -929,7 +973,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -940,7 +984,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -951,7 +995,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -962,7 +1006,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -973,7 +1017,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -984,7 +1028,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -995,7 +1039,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -1006,7 +1050,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -1017,7 +1061,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -1028,7 +1072,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -1039,7 +1083,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -1050,7 +1094,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -1061,7 +1105,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -1072,7 +1116,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -1083,7 +1127,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -1094,7 +1138,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -1105,7 +1149,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -1115,8 +1159,11 @@
       <c r="C43" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -1127,7 +1174,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -1138,7 +1185,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -1149,7 +1196,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -1167,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1178,9 +1225,11 @@
     <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -1190,8 +1239,14 @@
       <c r="C1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -1199,7 +1254,21 @@
         <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>102</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: front end ajust
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="geral" sheetId="1" r:id="rId1"/>
     <sheet name="segregados" sheetId="2" r:id="rId2"/>
+    <sheet name="erros" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="106">
   <si>
     <t>processo</t>
   </si>
@@ -335,6 +336,18 @@
   </si>
   <si>
     <t>Emissão de NF de Incineração (NFI)</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>DEV01</t>
+  </si>
+  <si>
+    <t>Saldo não é igual a zero: xxx,xx débito: xxx,xx Crédito: xxx,xx</t>
+  </si>
+  <si>
+    <t>erro</t>
   </si>
 </sst>
 </file>
@@ -657,7 +670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1260,4 +1273,39 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="51.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
build: ajust prompt ai
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640"/>
   </bookViews>
   <sheets>
     <sheet name="geral" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="110">
   <si>
     <t>processo</t>
   </si>
@@ -348,6 +348,18 @@
   </si>
   <si>
     <t>erro</t>
+  </si>
+  <si>
+    <t>MI31</t>
+  </si>
+  <si>
+    <t>Batch Input: criar doc.invent.</t>
+  </si>
+  <si>
+    <t>inventario</t>
+  </si>
+  <si>
+    <t>criação de documento de inventário</t>
   </si>
 </sst>
 </file>
@@ -668,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1204,6 +1216,20 @@
       </c>
       <c r="C46" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" t="s">
+        <v>108</v>
+      </c>
+      <c r="D47" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1279,7 +1305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: change in prompt in process
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="geral" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="115">
   <si>
     <t>processo</t>
   </si>
@@ -360,6 +360,21 @@
   </si>
   <si>
     <t>criação de documento de inventário</t>
+  </si>
+  <si>
+    <t>DEV02</t>
+  </si>
+  <si>
+    <t>DEV03</t>
+  </si>
+  <si>
+    <t>"Sem saldo para classificar/determinar","Material/Saldo sem NFO"</t>
+  </si>
+  <si>
+    <t>MR8M</t>
+  </si>
+  <si>
+    <t>Id não retornada a zsgr_100 após estorno de pedido na ME22N</t>
   </si>
 </sst>
 </file>
@@ -682,7 +697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
@@ -1303,31 +1318,59 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="51.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>102</v>
       </c>
       <c r="B1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
build: change prompt for subjects
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -12,10 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="geral" sheetId="1" r:id="rId1"/>
-    <sheet name="chamados" sheetId="4" r:id="rId2"/>
-    <sheet name="segregados" sheetId="2" r:id="rId3"/>
-    <sheet name="erros" sheetId="3" r:id="rId4"/>
+    <sheet name="chamados" sheetId="4" r:id="rId1"/>
+    <sheet name="geral" sheetId="1" r:id="rId2"/>
+    <sheet name="erros" sheetId="3" r:id="rId3"/>
+    <sheet name="segregados" sheetId="2" r:id="rId4"/>
+    <sheet name="recebimento" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -59,9 +60,6 @@
     <t>ERROSAP01</t>
   </si>
   <si>
-    <t>Avarias - Processo de avaria no CD</t>
-  </si>
-  <si>
     <t>Devolução fornecedor</t>
   </si>
   <si>
@@ -150,6 +148,9 @@
   </si>
   <si>
     <t>ERROSAP02</t>
+  </si>
+  <si>
+    <t>Processo de Avarias</t>
   </si>
 </sst>
 </file>
@@ -468,125 +469,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -604,39 +486,39 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1">
         <v>45627</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -644,22 +526,141 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1">
         <v>45627</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -669,74 +670,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -771,17 +707,94 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add tesseract to analyze images with ai
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640"/>
   </bookViews>
   <sheets>
     <sheet name="chamados" sheetId="4" r:id="rId1"/>
@@ -469,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -544,8 +544,12 @@
         <v>37</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -726,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>